<commit_message>
fixes and error handling
</commit_message>
<xml_diff>
--- a/linkedin_events.xlsx
+++ b/linkedin_events.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Event Name</t>
   </si>
@@ -31,104 +31,107 @@
     <t>Number of Attendees</t>
   </si>
   <si>
-    <t>🤯 HubSpot x LinkedIn Sales Nav x LinkedIn ads 👈 Ultimate ABM setup</t>
-  </si>
-  <si>
-    <t>Why HubSpot Content Hub is the best platform for B2B Websites</t>
-  </si>
-  <si>
-    <t>Top 10 Email Marketing &amp; Sales Trends</t>
-  </si>
-  <si>
-    <t>Hubspot CRM</t>
-  </si>
-  <si>
-    <t>HubSpot + Apollo.io for Super Powered Outbound</t>
-  </si>
-  <si>
-    <t>Inbox Impact: Email Mastery with HubSpot</t>
-  </si>
-  <si>
-    <t>Hubspot Quotes VS DealHub CPQ - A practical CPQ Comparison for HubSpot User</t>
-  </si>
-  <si>
-    <t>SEO for Revenue: Surviving &amp; Thriving In Google's Shift to Generative AI</t>
-  </si>
-  <si>
-    <t>Lead Object for Businesses: Which is better? Salesforce Vs. HubSpot</t>
-  </si>
-  <si>
-    <t>Tue, Jun 18, 2024, 7:00 PM - 8:00 PM (your local time)</t>
-  </si>
-  <si>
-    <t>Mon, Jun 17, 2024, 8:00 PM - 9:00 PM (your local time)</t>
-  </si>
-  <si>
-    <t>Fri, Jun 14, 2024, 10:00 PM (your local time)</t>
-  </si>
-  <si>
-    <t>Sun, Jun 30, 2024, 10:00 AM - 8:00 PM (your local time)</t>
-  </si>
-  <si>
-    <t>Fri, Jun 14, 2024, 1:30 AM - 2:00 AM (your local time)</t>
-  </si>
-  <si>
-    <t>Thu, Jun 27, 2024, 5:30 PM - 6:30 PM (your local time)</t>
-  </si>
-  <si>
-    <t>Tue, Jun 18, 2024, 3:00 PM - 3:45 PM (your local time)</t>
-  </si>
-  <si>
-    <t>Jun 20, 2024, 11:00 PM - Jun 21, 2024, 12:00 AM (your local time)</t>
-  </si>
-  <si>
-    <t>Thu, Jul 11, 2024, 9:00 PM - 9:30 PM (your local time)</t>
-  </si>
-  <si>
-    <t>Wouter Dieleman</t>
-  </si>
-  <si>
-    <t>Blend | The HubSpot Website Agency</t>
-  </si>
-  <si>
-    <t>INBOUND</t>
-  </si>
-  <si>
-    <t>Natalia Skachkova</t>
-  </si>
-  <si>
-    <t>Growth</t>
-  </si>
-  <si>
-    <t>Velocity</t>
-  </si>
-  <si>
-    <t>Elixir</t>
-  </si>
-  <si>
-    <t>Fire&amp;Spark</t>
-  </si>
-  <si>
-    <t>RevOps Automated</t>
-  </si>
-  <si>
-    <t>67 attendees</t>
-  </si>
-  <si>
-    <t>13 attendees</t>
-  </si>
-  <si>
-    <t>867 attendees</t>
-  </si>
-  <si>
-    <t>99 attendees</t>
+    <t>The future of AI Translation: LLMs or Neural MT? feat. João Graça</t>
+  </si>
+  <si>
+    <t>AI Insights: Part 3 - LLMs: Considerations When Choosing an LLM</t>
+  </si>
+  <si>
+    <t>Unlocking Enterprise Potential: Harnessing Open Source LLMs for Production</t>
+  </si>
+  <si>
+    <t>AI (LLMs) and XR Powered Digital Twins in Healthcare</t>
+  </si>
+  <si>
+    <t>Mastering Data Science: The Impact of LLMs</t>
+  </si>
+  <si>
+    <t>AI Governance: Data minimisation &amp; anonymisation while leveraging LLMs</t>
+  </si>
+  <si>
+    <t>How to align LLMs to enterprise objectives/policies</t>
+  </si>
+  <si>
+    <t>Pre-Training LLMs on Personal Computers</t>
+  </si>
+  <si>
+    <t>Building trustworthiness in AI using RAG</t>
+  </si>
+  <si>
+    <t>Hybrid Chatbots: Merging LLMs and Classification Models</t>
+  </si>
+  <si>
+    <t>Wed, Jun 26, 2024, 7:00 PM - 8:00 PM (your local time)</t>
+  </si>
+  <si>
+    <t>Wed, Jun 19, 2024, 12:00 AM (your local time)</t>
+  </si>
+  <si>
+    <t>Thu, Jun 20, 2024, 8:30 PM - 9:30 PM (your local time)</t>
+  </si>
+  <si>
+    <t>Wed, Jun 19, 2024, 9:00 PM - 10:00 PM (your local time)</t>
+  </si>
+  <si>
+    <t>Wed, Jul 17, 2024, 10:00 PM (your local time)</t>
+  </si>
+  <si>
+    <t>Thu, Jun 20, 2024, 6:00 PM - 6:30 PM (your local time)</t>
+  </si>
+  <si>
+    <t>Jun 18, 2024, 10:00 PM - Jun 19, 2024, 11:00 AM (your local time)</t>
+  </si>
+  <si>
+    <t>Wed, Aug 28, 2024, 9:00 PM (your local time)</t>
+  </si>
+  <si>
+    <t>Wed, Jun 26, 2024, 9:30 AM (your local time)</t>
+  </si>
+  <si>
+    <t>Wed, Aug 21, 2024, 10:00 PM (your local time)</t>
+  </si>
+  <si>
+    <t>Nimdzi Insights</t>
+  </si>
+  <si>
+    <t>Domo</t>
+  </si>
+  <si>
+    <t>WalkingTree Technologies</t>
+  </si>
+  <si>
+    <t>Alex G. Lee, Ph.D. Esq.</t>
+  </si>
+  <si>
+    <t>Data Science Dojo</t>
+  </si>
+  <si>
+    <t>TrustWorks</t>
+  </si>
+  <si>
+    <t>Snorkel AI</t>
+  </si>
+  <si>
+    <t>Katonic AI</t>
+  </si>
+  <si>
+    <t>https://us02web.zoom.us/webinar/register/WN_h5C6V61vSruKKCfWd8_nIQ</t>
+  </si>
+  <si>
+    <t>https://snorkel.ai/event/how-to-align-llms-to-enterprise-objectives-policies/</t>
+  </si>
+  <si>
+    <t>220 attendees</t>
+  </si>
+  <si>
+    <t>92 attendees</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +146,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -177,16 +187,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -479,7 +495,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -507,10 +523,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -518,10 +534,10 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -529,10 +545,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -540,10 +562,10 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -551,13 +573,10 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -565,10 +584,10 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -576,13 +595,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -590,13 +612,10 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -604,16 +623,28 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1"/>
+    <hyperlink ref="D8" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>